<commit_message>
editing user excel sheet
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -11,10 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Users</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Helen</t>
   </si>
@@ -47,18 +44,28 @@
   </si>
   <si>
     <t>Stephanie</t>
+  </si>
+  <si>
+    <t>Yung</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Anonymous</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
@@ -78,11 +85,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -306,59 +316,84 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding more users + removing unused variable
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>Helen</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Anna</t>
+  </si>
+  <si>
+    <t>Serge</t>
   </si>
   <si>
     <t>Anonymous</t>
@@ -1236,7 +1239,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1432,7 +1435,7 @@
     </row>
     <row r="21" ht="13.65" customHeight="1">
       <c r="A21" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1441,7 +1444,7 @@
     </row>
     <row r="22" ht="13.65" customHeight="1">
       <c r="A22" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1450,7 +1453,7 @@
     </row>
     <row r="23" ht="13.65" customHeight="1">
       <c r="A23" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1459,12 +1462,21 @@
     </row>
     <row r="24" ht="13.65" customHeight="1">
       <c r="A24" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
+    </row>
+    <row r="25" ht="13.65" customHeight="1">
+      <c r="A25" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>